<commit_message>
Styles for site header, logo, global nag, site name and site slogan. Update timesheet
</commit_message>
<xml_diff>
--- a/documents/timesheet/anthonyalbertyn-timesheet.xlsx
+++ b/documents/timesheet/anthonyalbertyn-timesheet.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>DATE</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Improve semantic markup, debug broken markup, imrpve semantic markup and make markup pass HTML 5 validation checks, introduce more mobile responsive behaviour to the page layout.</t>
+  </si>
+  <si>
+    <t>Start styling page header. logo, global menu, site name, site slogan, global header and local header.</t>
   </si>
 </sst>
 </file>
@@ -93,6 +96,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -491,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -581,6 +585,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2">
+        <v>41986</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Styling for header, main menu, mobile responsive styling for global nav and main nav, styles for page text like page headings, standfirst, secondary headings and paragraphs. Update timesheet.
</commit_message>
<xml_diff>
--- a/documents/timesheet/anthonyalbertyn-timesheet.xlsx
+++ b/documents/timesheet/anthonyalbertyn-timesheet.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>DATE</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Start styling page header. logo, global menu, site name, site slogan, global header and local header.</t>
+  </si>
+  <si>
+    <t>Styling for header, main menu, mobile responsive styling for global nav and main nav, styles for page text like page headings, standfirst, secondary headings and paragraphs.</t>
   </si>
 </sst>
 </file>
@@ -495,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -596,6 +599,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="9" spans="1:3" ht="30">
+      <c r="A9" s="2">
+        <v>41987</v>
+      </c>
+      <c r="B9" s="3">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updating time sheets for work done on 22/11/2014
</commit_message>
<xml_diff>
--- a/documents/timesheet/anthonyalbertyn-timesheet.xlsx
+++ b/documents/timesheet/anthonyalbertyn-timesheet.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>DATE</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Total cost £</t>
+  </si>
+  <si>
+    <t>Footer navigation and mobile responsive behavior for footer.</t>
   </si>
 </sst>
 </file>
@@ -522,7 +525,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -611,7 +614,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2">
-        <v>41986</v>
+        <v>41956</v>
       </c>
       <c r="B8" s="3">
         <v>2.1</v>
@@ -622,7 +625,7 @@
     </row>
     <row r="9" spans="1:3" ht="30">
       <c r="A9" s="2">
-        <v>41987</v>
+        <v>41957</v>
       </c>
       <c r="B9" s="3">
         <v>3</v>
@@ -633,13 +636,24 @@
     </row>
     <row r="10" spans="1:3" ht="30">
       <c r="A10" s="2">
-        <v>41988</v>
+        <v>41957</v>
       </c>
       <c r="B10" s="3">
         <v>5.17</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2">
+        <v>41965</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -648,7 +662,7 @@
       </c>
       <c r="B28" s="9">
         <f>SUM(B2:B27)</f>
-        <v>29.990000000000002</v>
+        <v>32.49</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -657,7 +671,7 @@
       </c>
       <c r="B29" s="9">
         <f>B28*45</f>
-        <v>1349.5500000000002</v>
+        <v>1462.0500000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>